<commit_message>
Added Super model metrics tables and t-test tables
</commit_message>
<xml_diff>
--- a/article/tables/t_Test_Results_Analysis_07-Jul-2023.xlsx
+++ b/article/tables/t_Test_Results_Analysis_07-Jul-2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rajesh\ResearchLab\RL_for_PdM\REINFORCE_Tool_Replace_Policy\results\07-Jul-2023_Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResearchLab\Empirical_Study_REINFORCE\article\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD10A0D-27C8-4A61-8DF7-6029C87F5405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3A2621-C731-4658-851C-AB43E07AC22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="267" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="267" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="t_Test_Results_csv_07-Jul-2023" sheetId="1" r:id="rId1"/>
@@ -1195,18 +1195,18 @@
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="15" max="15" width="48.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="15" max="15" width="48.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1438,7 +1438,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2143,7 +2143,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2963,59 +2963,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:Q31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="4.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
     <col min="9" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="4.5703125" customWidth="1"/>
+    <col min="12" max="12" width="4.5546875" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="18" width="11" customWidth="1"/>
     <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="12" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="12" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="33" max="34" width="12" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="11" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="12" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="38" max="39" width="12" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="7" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="12" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="46" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>70</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
         <v>67</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>68</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>69</v>
       </c>
@@ -3047,20 +3047,20 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="G8" s="12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="G9" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
     </row>
-    <row r="11" spans="2:17" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" s="10" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>60</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="2:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="s">
         <v>64</v>
@@ -3110,7 +3110,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>14</v>
       </c>
@@ -3133,7 +3133,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>0.60915655188727502</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
@@ -3219,7 +3219,7 @@
         <v>0.68676149346608695</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>0.62919999999999998</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="1"/>
@@ -3279,7 +3279,7 @@
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>51</v>
       </c>
@@ -3304,7 +3304,7 @@
       <c r="P18" s="4"/>
       <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>42</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>0.84138310023543705</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>0.80587057999512901</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>31</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>0.915333333333333</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
@@ -3450,7 +3450,7 @@
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>52</v>
       </c>
@@ -3475,7 +3475,7 @@
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>0.56982111049793405</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
@@ -3561,7 +3561,7 @@
         <v>0.60503064802476902</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>31</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>0.60333333333333306</v>
       </c>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="1"/>
@@ -3621,7 +3621,7 @@
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="3" t="s">
         <v>53</v>
       </c>
@@ -3646,7 +3646,7 @@
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>42</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>0.49493632770713403</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>18</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>0.81284494326099799</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>31</v>
       </c>

</xml_diff>